<commit_message>
Changes to be committed: 	modified:   Assignments/rmcmilan1MoEPoFS.xlsx 	new file:   Assignments/rmcmillan1MoEPoFSpace.docx
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>LINEST OUTPUT</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>&lt;- uncert of y-int</t>
+  </si>
+  <si>
+    <t>1/r (1/Distance)</t>
+  </si>
+  <si>
+    <t>C/(3.14*Distance*Distance)</t>
   </si>
 </sst>
 </file>
@@ -147,6 +153,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Distance vs. Capacitance</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -582,12 +613,312 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Capacitance/Area</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.7491225789678917E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4928343949044586E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7692852087756547E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1019108280254776E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2898352371427066E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.2779547062986558E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="572108872"/>
+        <c:axId val="202074832"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="572108872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="202074832"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="202074832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="572108872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -650,6 +981,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1166,20 +1537,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>57149</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>962024</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1193,6 +2080,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1204912</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1701355</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>101155</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1464,10 +2381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1476,9 +2393,10 @@
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1488,56 +2406,110 @@
       <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>7</v>
       </c>
       <c r="C2">
         <v>1.5</v>
       </c>
+      <c r="D2">
+        <f>1/B2</f>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="E2">
+        <f>C2/(3.14*B2*B2)</f>
+        <v>9.7491225789678917E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>8</v>
       </c>
       <c r="C3">
         <v>3</v>
       </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D7" si="0">1/B3</f>
+        <v>0.125</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E7" si="1">C3/(3.14*B3*B3)</f>
+        <v>1.4928343949044586E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>9</v>
       </c>
       <c r="C4">
         <v>4.5</v>
       </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>1.7692852087756547E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>10</v>
       </c>
       <c r="C5">
         <v>6.6</v>
       </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>2.1019108280254776E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>11</v>
       </c>
       <c r="C6">
         <v>8.6999999999999993</v>
       </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>9.0909090909090912E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>2.2898352371427066E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>12</v>
       </c>
       <c r="C7">
         <v>10.3</v>
       </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>2.2779547062986558E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
@@ -1546,7 +2518,7 @@
         <v>1.2523809523809515</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -1554,7 +2526,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -1569,7 +2541,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
@@ -1583,7 +2555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1597,7 +2569,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1609,7 +2581,7 @@
       </c>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16">
         <v>57.060571428571436</v>

</xml_diff>

<commit_message>
update to picoFarads  Changes to be committed: 	modified:   LAB/Assignments/rmcmilan1MoEPoFS.xlsx 	modified:   LAB/Assignments/rmcmillan1MoEPoFSpace.docx 	modified:   LAB/Assignments/rmcmillan1MoEPoFSpace.pdf
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
@@ -41,9 +41,6 @@
     <t>Distance (mm) x</t>
   </si>
   <si>
-    <t>Capacitance (Farads) y</t>
-  </si>
-  <si>
     <t>R^2 -&gt;</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>C/(3.14*Distance*Distance)</t>
+  </si>
+  <si>
+    <t>Capacitance (picoFarads) y</t>
   </si>
 </sst>
 </file>
@@ -358,11 +358,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="557885440"/>
-        <c:axId val="557885048"/>
+        <c:axId val="649782560"/>
+        <c:axId val="649782952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="557885440"/>
+        <c:axId val="649782560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,12 +475,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="557885048"/>
+        <c:crossAx val="649782952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="557885048"/>
+        <c:axId val="649782952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -592,312 +592,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="557885440"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Capacitance/Area</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$E$2:$E$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.7491225789678917E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.4928343949044586E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.7692852087756547E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.1019108280254776E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.2898352371427066E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.2779547062986558E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="572108872"/>
-        <c:axId val="202074832"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="572108872"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="202074832"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="202074832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="572108872"/>
+        <c:crossAx val="649782560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -981,563 +676,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2063,10 +1202,10 @@
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>962024</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2080,36 +1219,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1204912</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1701355</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>101155</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2383,34 +1492,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -2511,7 +1620,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="1">
         <f>$B$12*B2+$C$12</f>
@@ -2552,12 +1661,12 @@
         <v>0.58001211966381916</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14">
         <v>0.99558982369265026</v>
@@ -2566,12 +1675,12 @@
         <v>0.25137715924577608</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>902.99321778447541</v>

</xml_diff>

<commit_message>
Changes to be committed: 	modified:   LAB/Assignments/rmcmilan1MoEPoFS.xlsx
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>LINEST OUTPUT</t>
   </si>
@@ -62,10 +62,10 @@
     <t>1/r (1/Distance)</t>
   </si>
   <si>
-    <t>C/(3.14*Distance*Distance)</t>
+    <t>Capacitance (picoFarads) y</t>
   </si>
   <si>
-    <t>Capacitance (picoFarads) y</t>
+    <t>C/(3.14*radius*radius)</t>
   </si>
 </sst>
 </file>
@@ -153,31 +153,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Distance vs. Capacitance</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -239,111 +214,56 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
-            <c:noEndCap val="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$9</c:f>
+              <c:f>Sheet1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.2523809523809515</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$9</c:f>
+              <c:f>Sheet1!$C$2:$C$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>1.5000000000000001E-12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0000000000000001E-12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5</c:v>
+                  <c:v>4.4999999999999998E-12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6</c:v>
+                  <c:v>6.5999999999999993E-12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6999999999999993</c:v>
+                  <c:v>8.6999999999999997E-12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.3</c:v>
+                  <c:v>1.0300000000000001E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,11 +278,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="649782560"/>
-        <c:axId val="649782952"/>
+        <c:axId val="636821648"/>
+        <c:axId val="636822824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="649782560"/>
+        <c:axId val="636821648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -382,62 +302,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Distance (mm)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -475,12 +339,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649782952"/>
+        <c:crossAx val="636822824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="649782952"/>
+        <c:axId val="636822824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -490,8 +354,9 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="accent1">
-                  <a:alpha val="50000"/>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -499,62 +364,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Capacitance (Farads)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -592,7 +401,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="649782560"/>
+        <c:crossAx val="636821648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -613,7 +422,324 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>14.285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.0909090909090917</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.3333333333333339</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.1942675159235668E-11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3885350318471336E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5828025477706999E-11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2547770700636933E-11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9267515923566868E-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2006369426751591E-11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="636823216"/>
+        <c:axId val="636826352"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="636823216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="636826352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="636826352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="636823216"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -676,6 +802,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1192,24 +1358,540 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>14286</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323849</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1219,6 +1901,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1714499</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1490,10 +2202,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,109 +2225,121 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2">
-        <v>7</v>
+        <f>7*10^-2</f>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C2">
-        <v>1.5</v>
+        <f>1.5*10^-12</f>
+        <v>1.5000000000000001E-12</v>
       </c>
       <c r="D2">
         <f>1/B2</f>
-        <v>0.14285714285714285</v>
+        <v>14.285714285714285</v>
       </c>
       <c r="E2">
-        <f>C2/(3.14*B2*B2)</f>
-        <v>9.7491225789678917E-3</v>
+        <f>C2/(3.14*0.2*0.2)</f>
+        <v>1.1942675159235668E-11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3">
-        <v>8</v>
+        <f>8*10^-2</f>
+        <v>0.08</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <f>3*10^-12</f>
+        <v>3.0000000000000001E-12</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D7" si="0">1/B3</f>
-        <v>0.125</v>
+        <v>12.5</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E7" si="1">C3/(3.14*B3*B3)</f>
-        <v>1.4928343949044586E-2</v>
+        <f t="shared" ref="E3:E7" si="1">C3/(3.14*0.2*0.2)</f>
+        <v>2.3885350318471336E-11</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
-        <v>9</v>
+        <f>9*10^-2</f>
+        <v>0.09</v>
       </c>
       <c r="C4">
-        <v>4.5</v>
+        <f>4.5*10^-12</f>
+        <v>4.4999999999999998E-12</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
+        <v>11.111111111111111</v>
       </c>
       <c r="E4">
         <f t="shared" si="1"/>
-        <v>1.7692852087756547E-2</v>
+        <v>3.5828025477706999E-11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>10</v>
+        <f>10*10^-2</f>
+        <v>0.1</v>
       </c>
       <c r="C5">
-        <v>6.6</v>
+        <f>6.6*10^-12</f>
+        <v>6.5999999999999993E-12</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>10</v>
       </c>
       <c r="E5">
         <f t="shared" si="1"/>
-        <v>2.1019108280254776E-2</v>
+        <v>5.2547770700636933E-11</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>11</v>
+        <f>11*10^-2</f>
+        <v>0.11</v>
       </c>
       <c r="C6">
-        <v>8.6999999999999993</v>
+        <f>8.7*10^-12</f>
+        <v>8.6999999999999997E-12</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
+        <v>9.0909090909090917</v>
       </c>
       <c r="E6">
         <f t="shared" si="1"/>
-        <v>2.2898352371427066E-2</v>
+        <v>6.9267515923566868E-11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>12</v>
+        <f>12*10^-2</f>
+        <v>0.12</v>
       </c>
       <c r="C7">
-        <v>10.3</v>
+        <f>10.3*10^-12</f>
+        <v>1.0300000000000001E-11</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>2.2779547062986558E-2</v>
+        <v>8.2006369426751591E-11</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1624,7 +2348,7 @@
       </c>
       <c r="B9" s="1">
         <f>$B$12*B2+$C$12</f>
-        <v>1.2523809523809515</v>
+        <v>1.2523809523809506E-12</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1641,10 +2365,10 @@
       </c>
       <c r="B12">
         <f t="array" ref="B12:C16">LINEST(C2:C7,B2:B7,TRUE,TRUE)</f>
-        <v>1.8057142857142856</v>
+        <v>1.8057142857142862E-10</v>
       </c>
       <c r="C12">
-        <v>-11.387619047619047</v>
+        <v>-1.1387619047619054E-11</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
@@ -1655,10 +2379,10 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>6.0090634492751864E-2</v>
+        <v>6.0090634492751662E-12</v>
       </c>
       <c r="C13">
-        <v>0.58001211966381916</v>
+        <v>5.8001211966381726E-13</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
@@ -1669,10 +2393,10 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>0.99558982369265026</v>
+        <v>0.99558982369265037</v>
       </c>
       <c r="C14">
-        <v>0.25137715924577608</v>
+        <v>2.513771592457752E-13</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>8</v>
@@ -1683,7 +2407,7 @@
         <v>7</v>
       </c>
       <c r="B15">
-        <v>902.99321778447541</v>
+        <v>902.99321778448166</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -1693,12 +2417,85 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16">
-        <v>57.060571428571436</v>
+        <v>5.7060571428571438E-23</v>
       </c>
       <c r="C16">
-        <v>0.25276190476190502</v>
+        <v>2.527619047619033E-25</v>
       </c>
       <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18">
+        <f t="array" ref="B18:C22">LINEST(E2:E6,D2:D6,TRUE,TRUE)</f>
+        <v>-1.0799625478840946E-11</v>
+      </c>
+      <c r="C18">
+        <v>1.6178350538695559E-10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>1.3844709192482616E-12</v>
+      </c>
+      <c r="C19">
+        <v>1.5983691889901586E-11</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>0.95301375800992383</v>
+      </c>
+      <c r="C20">
+        <v>5.6936397217434394E-12</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>60.848477191123841</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22">
+        <v>1.9725575344423217E-21</v>
+      </c>
+      <c r="C22">
+        <v>9.7252599843044139E-23</v>
+      </c>
+      <c r="D22" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes to be committed: 	new file:   LAB/Assignments/DATA.docx 	modified:   LAB/Assignments/rmcmilan1MoEPoFS.xlsx 	new file:   LAB/Assignments/rmcmilan1MoEPoFSExcel.pdf
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
@@ -153,6 +153,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DATA collection</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -423,12 +448,7 @@
       <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -466,6 +486,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>DATA Analysis</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -736,12 +781,7 @@
       <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1888,14 +1928,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>14286</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1409699</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>323849</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4581524</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1918,16 +1958,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1714499</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>4571999</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>180976</xdr:rowOff>
+      <xdr:rowOff>171451</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2215,7 +2255,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2225,6 +2265,7 @@
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="68.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
new file:   Is the Sun DISINTEGRATING? NASA spots monster hole open up on our star | Science | News | Daily Express.pdf         modified:   LAB/Assignments/rmcmilan1MoEPoFS.xlsx
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
@@ -1961,13 +1961,13 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>9524</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>4571999</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2255,7 +2255,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
something is working here... 	modified:   LAB/Assignments/rmcmilan1MoEPoFS.xlsx
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>LINEST OUTPUT</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>&lt;- y intercept</t>
-  </si>
-  <si>
-    <t>Distance (mm) x</t>
   </si>
   <si>
     <t>R^2 -&gt;</t>
@@ -53,19 +50,25 @@
     <t>&lt;- Variance</t>
   </si>
   <si>
-    <t>Fit -&gt;</t>
-  </si>
-  <si>
     <t>&lt;- uncert of y-int</t>
   </si>
   <si>
     <t>Capacitance (picoFarads) y</t>
   </si>
   <si>
-    <t>C/(3.14*radius*radius)</t>
+    <t>Distance (meters) x</t>
   </si>
   <si>
-    <t>1/Distance</t>
+    <t>y = C/(3.14*radius*radius)</t>
+  </si>
+  <si>
+    <t>x = 1/Distance</t>
+  </si>
+  <si>
+    <t>Fit1 -&gt;</t>
+  </si>
+  <si>
+    <t>Fit2 -&gt;</t>
   </si>
 </sst>
 </file>
@@ -173,7 +176,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>DATA collection</a:t>
+              <a:t>DATA collection C vs. x</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -247,22 +250,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -274,22 +277,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.5</c:v>
+                  <c:v>1.5000000000000001E-12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>3.0000000000000001E-12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5</c:v>
+                  <c:v>4.4999999999999998E-12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.6</c:v>
+                  <c:v>6.5999999999999993E-12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6999999999999993</c:v>
+                  <c:v>8.6999999999999997E-12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.3</c:v>
+                  <c:v>1.0300000000000001E-11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -304,11 +307,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="636821648"/>
-        <c:axId val="636822824"/>
+        <c:axId val="392189496"/>
+        <c:axId val="392282624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="636821648"/>
+        <c:axId val="392189496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -365,12 +368,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636822824"/>
+        <c:crossAx val="392282624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="636822824"/>
+        <c:axId val="392282624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -427,7 +430,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636821648"/>
+        <c:crossAx val="392189496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -580,22 +583,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>0.14285714285714285</c:v>
+                  <c:v>14.285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.125</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1111111111111111</c:v>
+                  <c:v>11.111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.0909090909090912E-2</c:v>
+                  <c:v>9.0909090909090917</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.3333333333333329E-2</c:v>
+                  <c:v>8.3333333333333339</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -607,22 +610,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>191.08280254777068</c:v>
+                  <c:v>1.9108280254777069E-10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>382.16560509554137</c:v>
+                  <c:v>3.8216560509554138E-10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>573.24840764331202</c:v>
+                  <c:v>5.7324840764331199E-10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>840.7643312101909</c:v>
+                  <c:v>8.4076433121019094E-10</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1108.2802547770698</c:v>
+                  <c:v>1.1082802547770699E-9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1312.1019108280254</c:v>
+                  <c:v>1.3121019108280255E-9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -637,11 +640,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="636823216"/>
-        <c:axId val="636826352"/>
+        <c:axId val="392283408"/>
+        <c:axId val="392283800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="636823216"/>
+        <c:axId val="392283408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -698,12 +701,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636826352"/>
+        <c:crossAx val="392283800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="636826352"/>
+        <c:axId val="392283800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -760,7 +763,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="636823216"/>
+        <c:crossAx val="392283408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1928,14 +1931,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1409699</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>4581524</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1959,13 +1962,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:colOff>47624</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>85726</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>4571999</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>66676</xdr:rowOff>
     </xdr:to>
@@ -2255,157 +2258,160 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="68.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2">
-        <f>7*10^0</f>
-        <v>7</v>
+        <f>7*10^-2</f>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C2">
-        <f>1.5*10^0</f>
-        <v>1.5</v>
+        <f>1.5*10^-12</f>
+        <v>1.5000000000000001E-12</v>
       </c>
       <c r="D2">
         <f>1/(B2*10^0)</f>
-        <v>0.14285714285714285</v>
+        <v>14.285714285714285</v>
       </c>
       <c r="E2">
-        <f>C2/(3.14*0.05*0.05)</f>
-        <v>191.08280254777068</v>
+        <f t="shared" ref="E2:E7" si="0">C2/(3.14*0.05*0.05)</f>
+        <v>1.9108280254777069E-10</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3">
-        <f>8*10^0</f>
-        <v>8</v>
+        <f>8*10^-2</f>
+        <v>0.08</v>
       </c>
       <c r="C3">
-        <f>3*10^0</f>
-        <v>3</v>
+        <f>3*10^-12</f>
+        <v>3.0000000000000001E-12</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D7" si="0">1/(B3*10^0)</f>
-        <v>0.125</v>
+        <f t="shared" ref="D3:D7" si="1">1/(B3*10^0)</f>
+        <v>12.5</v>
       </c>
       <c r="E3">
-        <f>C3/(3.14*0.05*0.05)</f>
-        <v>382.16560509554137</v>
+        <f t="shared" si="0"/>
+        <v>3.8216560509554138E-10</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
-        <f>9*10^0</f>
-        <v>9</v>
+        <f>9*10^-2</f>
+        <v>0.09</v>
       </c>
       <c r="C4">
-        <f>4.5*10^0</f>
-        <v>4.5</v>
+        <f>4.5*10^-12</f>
+        <v>4.4999999999999998E-12</v>
       </c>
       <c r="D4">
+        <f t="shared" si="1"/>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="E4">
         <f t="shared" si="0"/>
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="E4">
-        <f>C4/(3.14*0.05*0.05)</f>
-        <v>573.24840764331202</v>
+        <v>5.7324840764331199E-10</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
-        <f>10*10^0</f>
+        <f>10*10^-2</f>
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <f>6.6*10^-12</f>
+        <v>6.5999999999999993E-12</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="C5">
-        <f>6.6*10^0</f>
-        <v>6.6</v>
-      </c>
-      <c r="D5">
+      <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="E5">
-        <f>C5/(3.14*0.05*0.05)</f>
-        <v>840.7643312101909</v>
+        <v>8.4076433121019094E-10</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
-        <f>11*10^0</f>
-        <v>11</v>
+        <f>11*10^-2</f>
+        <v>0.11</v>
       </c>
       <c r="C6">
-        <f>8.7*10^0</f>
-        <v>8.6999999999999993</v>
+        <f>8.7*10^-12</f>
+        <v>8.6999999999999997E-12</v>
       </c>
       <c r="D6">
+        <f t="shared" si="1"/>
+        <v>9.0909090909090917</v>
+      </c>
+      <c r="E6">
         <f t="shared" si="0"/>
-        <v>9.0909090909090912E-2</v>
-      </c>
-      <c r="E6">
-        <f>C6/(3.14*0.05*0.05)</f>
-        <v>1108.2802547770698</v>
+        <v>1.1082802547770699E-9</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
-        <f>12*10^0</f>
-        <v>12</v>
+        <f>12*10^-2</f>
+        <v>0.12</v>
       </c>
       <c r="C7">
-        <f>10.3*10^0</f>
-        <v>10.3</v>
+        <f>10.3*10^-12</f>
+        <v>1.0300000000000001E-11</v>
       </c>
       <c r="D7">
+        <f t="shared" si="1"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>8.3333333333333329E-2</v>
-      </c>
-      <c r="E7">
-        <f>C7/(3.14*0.05*0.05)</f>
-        <v>1312.1019108280254</v>
+        <v>1.3121019108280255E-9</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <f>$B$12*B2+$C$12</f>
-        <v>1.2523809523809515</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>1.2523809523809506E-12</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D9" s="1">
-        <f>$B$18*B2+$C$18</f>
-        <v>-129971.58082969925</v>
-      </c>
+        <f>$B$18*D2+$C$18</f>
+        <v>8.9933275051011534E-11</v>
+      </c>
+      <c r="E9" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -2421,10 +2427,10 @@
       </c>
       <c r="B12">
         <f t="array" ref="B12:C16">LINEST(C2:C7,B2:B7,TRUE,TRUE)</f>
-        <v>1.8057142857142856</v>
+        <v>1.8057142857142862E-10</v>
       </c>
       <c r="C12">
-        <v>-11.387619047619047</v>
+        <v>-1.1387619047619054E-11</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
@@ -2435,35 +2441,35 @@
         <v>2</v>
       </c>
       <c r="B13">
-        <v>6.0090634492751864E-2</v>
+        <v>6.0090634492751662E-12</v>
       </c>
       <c r="C13">
-        <v>0.58001211966381916</v>
+        <v>5.8001211966381726E-13</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14">
-        <v>0.99558982369265026</v>
+        <v>0.99558982369265037</v>
       </c>
       <c r="C14">
-        <v>0.25137715924577608</v>
+        <v>2.513771592457752E-13</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15">
-        <v>902.99321778447541</v>
+        <v>902.99321778448166</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -2473,10 +2479,10 @@
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16">
-        <v>57.060571428571436</v>
+        <v>5.7060571428571438E-23</v>
       </c>
       <c r="C16">
-        <v>0.25276190476190502</v>
+        <v>2.527619047619033E-25</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -2494,10 +2500,10 @@
       </c>
       <c r="B18">
         <f t="array" ref="B18:C22">LINEST(E2:E7,D2:D7,TRUE,TRUE)</f>
-        <v>-18967.304140276079</v>
+        <v>-1.8967304140276085E-10</v>
       </c>
       <c r="C18">
-        <v>2799.5481522333089</v>
+        <v>2.7995481522333092E-9</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>3</v>
@@ -2508,35 +2514,35 @@
         <v>2</v>
       </c>
       <c r="B19">
-        <v>2013.8661785306717</v>
+        <v>2.0138661785306717E-11</v>
       </c>
       <c r="C19">
-        <v>223.02715470024768</v>
+        <v>2.2302715470024771E-10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>0.95685256178327316</v>
       </c>
       <c r="C20">
-        <v>100.16262303254362</v>
+        <v>1.001626230325436E-10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21">
-        <v>88.705387974791208</v>
+        <v>88.705387974791236</v>
       </c>
       <c r="C21">
         <v>4</v>
@@ -2546,10 +2552,10 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22">
-        <v>889941.33351192588</v>
+        <v>8.8994133351192587E-19</v>
       </c>
       <c r="C22">
-        <v>40130.204211037752</v>
+        <v>4.0130204211037735E-20</v>
       </c>
       <c r="D22" s="1"/>
     </row>

</xml_diff>

<commit_message>
modified:   LAB/Assignments/rmcmilan1MoEPoFS.xlsx         modified:   LAB/Assignments/rmcmillan1MoEPoFSpace2.docx
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
@@ -1381,7 +1381,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="F18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1549,8 +1549,8 @@
         <v>15</v>
       </c>
       <c r="D10">
-        <f>(B9-B10)/C14</f>
-        <v>1.3891459796929202E-3</v>
+        <f>(B9-B10)/B13</f>
+        <v>6.909123683812652E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
modified:   rmcmilan1MoEPoFS.xlsx 	modified:   rmcmillan1MoEPoFSpace2.docx 	modified:   rmcmillan1MoEPoFSpace2.pdf
</commit_message>
<xml_diff>
--- a/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
+++ b/LAB/Assignments/rmcmilan1MoEPoFS.xlsx
@@ -289,6 +289,44 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$2:$B$7</c:f>
@@ -353,11 +391,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="392189496"/>
-        <c:axId val="392282624"/>
+        <c:axId val="328799544"/>
+        <c:axId val="328799936"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="392189496"/>
+        <c:axId val="328799544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,12 +452,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392282624"/>
+        <c:crossAx val="328799936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="392282624"/>
+        <c:axId val="328799936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -476,7 +514,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="392189496"/>
+        <c:crossAx val="328799544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1380,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="F29" sqref="A1:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>